<commit_message>
updated metadata from Tauber
</commit_message>
<xml_diff>
--- a/populationInfo/OriginalMetadata/AOB.JCBN.Final Extraction data _Microgen_DrosEU_2017-2021.xlsx
+++ b/populationInfo/OriginalMetadata/AOB.JCBN.Final Extraction data _Microgen_DrosEU_2017-2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanbergland/Documents/work/Projects/2022_DESTv2/Metadata collection sheets/Finalized docs/Dec 15 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanbergland/Documents/GitHub/DESTv2/populationInfo/OriginalMetadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137A4AD0-0FF8-A54C-A58A-5DEB6443332A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C616DB-D7DA-024B-8F53-5D5D4D9A52BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="500" windowWidth="26200" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8140" yWindow="500" windowWidth="26200" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extraction " sheetId="6" r:id="rId1"/>
@@ -2905,7 +2905,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2957,6 +2957,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3404,7 +3410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3712,16 +3718,51 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4004,8 +4045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P254"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C261" sqref="C261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4057,7 +4098,7 @@
       <c r="K1" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="L1" s="131" t="s">
+      <c r="L1" s="130" t="s">
         <v>923</v>
       </c>
       <c r="M1" s="87" t="s">
@@ -7620,7 +7661,7 @@
       <c r="N85" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="O85" s="130" t="s">
+      <c r="O85" s="129" t="s">
         <v>920</v>
       </c>
     </row>
@@ -7663,7 +7704,7 @@
       <c r="N86" s="9" t="s">
         <v>831</v>
       </c>
-      <c r="O86" s="130" t="s">
+      <c r="O86" s="129" t="s">
         <v>920</v>
       </c>
     </row>
@@ -7790,7 +7831,7 @@
       <c r="N89" s="9" t="s">
         <v>837</v>
       </c>
-      <c r="O89" s="130" t="s">
+      <c r="O89" s="129" t="s">
         <v>62</v>
       </c>
     </row>
@@ -14565,183 +14606,183 @@
         <v>885</v>
       </c>
     </row>
-    <row r="251" spans="1:15" s="11" customFormat="1" ht="16" thickBot="1">
-      <c r="A251" s="13">
+    <row r="251" spans="1:15" s="136" customFormat="1" ht="16" thickBot="1">
+      <c r="A251" s="131">
         <v>176</v>
       </c>
-      <c r="B251" s="14" t="s">
+      <c r="B251" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="C251" s="14" t="s">
+      <c r="C251" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="D251" s="15" t="s">
+      <c r="D251" s="133" t="s">
         <v>183</v>
       </c>
-      <c r="E251" s="15">
+      <c r="E251" s="133">
         <v>2019</v>
       </c>
-      <c r="F251" s="14" t="s">
+      <c r="F251" s="132" t="s">
         <v>184</v>
       </c>
-      <c r="G251" s="14"/>
-      <c r="H251" s="14">
+      <c r="G251" s="132"/>
+      <c r="H251" s="132">
         <v>35</v>
       </c>
-      <c r="I251" s="14" t="s">
+      <c r="I251" s="132" t="s">
         <v>369</v>
       </c>
-      <c r="J251" s="14" t="s">
+      <c r="J251" s="132" t="s">
         <v>218</v>
       </c>
-      <c r="K251" s="14" t="s">
+      <c r="K251" s="132" t="s">
         <v>752</v>
       </c>
-      <c r="L251" s="73">
+      <c r="L251" s="134">
         <v>148</v>
       </c>
-      <c r="M251" s="128" t="s">
-        <v>912</v>
-      </c>
-      <c r="N251" s="14" t="s">
+      <c r="M251" s="135" t="s">
+        <v>912</v>
+      </c>
+      <c r="N251" s="132" t="s">
         <v>753</v>
       </c>
-      <c r="O251" s="11" t="s">
+      <c r="O251" s="136" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="252" spans="1:15" s="19" customFormat="1">
-      <c r="A252" s="18">
+    <row r="252" spans="1:15" s="143" customFormat="1">
+      <c r="A252" s="137">
         <v>181</v>
       </c>
-      <c r="B252" s="17" t="s">
+      <c r="B252" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="C252" s="17" t="s">
+      <c r="C252" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="D252" s="16" t="s">
+      <c r="D252" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="E252" s="16">
+      <c r="E252" s="139">
         <v>2019</v>
       </c>
-      <c r="F252" s="17" t="s">
+      <c r="F252" s="138" t="s">
         <v>184</v>
       </c>
-      <c r="G252" s="17"/>
-      <c r="H252" s="17">
+      <c r="G252" s="138"/>
+      <c r="H252" s="138">
         <v>38</v>
       </c>
-      <c r="I252" s="17" t="s">
+      <c r="I252" s="138" t="s">
         <v>369</v>
       </c>
-      <c r="J252" s="17" t="s">
+      <c r="J252" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="K252" s="17" t="s">
+      <c r="K252" s="138" t="s">
         <v>762</v>
       </c>
-      <c r="L252" s="108">
+      <c r="L252" s="140">
         <v>153</v>
       </c>
-      <c r="M252" s="129" t="s">
+      <c r="M252" s="141" t="s">
         <v>925</v>
       </c>
-      <c r="N252" s="17" t="s">
+      <c r="N252" s="138" t="s">
         <v>763</v>
       </c>
-      <c r="O252" s="132" t="s">
+      <c r="O252" s="142" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="253" spans="1:15" s="25" customFormat="1" ht="16" thickBot="1">
-      <c r="A253" s="21">
+    <row r="253" spans="1:15" s="147" customFormat="1" ht="16" thickBot="1">
+      <c r="A253" s="144">
         <v>224</v>
       </c>
-      <c r="B253" s="22" t="s">
+      <c r="B253" s="145" t="s">
         <v>66</v>
       </c>
-      <c r="C253" s="22" t="s">
+      <c r="C253" s="145" t="s">
         <v>67</v>
       </c>
-      <c r="D253" s="24" t="s">
+      <c r="D253" s="146" t="s">
         <v>81</v>
       </c>
-      <c r="E253" s="24">
+      <c r="E253" s="146">
         <v>2017</v>
       </c>
-      <c r="F253" s="22" t="s">
+      <c r="F253" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="G253" s="22"/>
-      <c r="H253" s="22">
-        <v>40</v>
-      </c>
-      <c r="I253" s="22" t="s">
+      <c r="G253" s="145"/>
+      <c r="H253" s="145">
+        <v>40</v>
+      </c>
+      <c r="I253" s="145" t="s">
         <v>369</v>
       </c>
-      <c r="J253" s="22" t="s">
+      <c r="J253" s="145" t="s">
         <v>210</v>
       </c>
-      <c r="K253" s="22" t="s">
+      <c r="K253" s="145" t="s">
         <v>848</v>
       </c>
-      <c r="L253" s="108">
+      <c r="L253" s="140">
         <v>94</v>
       </c>
-      <c r="M253" s="129" t="s">
+      <c r="M253" s="141" t="s">
         <v>925</v>
       </c>
-      <c r="N253" s="22" t="s">
+      <c r="N253" s="145" t="s">
         <v>849</v>
       </c>
-      <c r="O253" s="132" t="s">
+      <c r="O253" s="142" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="254" spans="1:15" s="11" customFormat="1">
-      <c r="A254" s="33">
+    <row r="254" spans="1:15" s="136" customFormat="1">
+      <c r="A254" s="148">
         <v>225</v>
       </c>
-      <c r="B254" s="34" t="s">
+      <c r="B254" s="149" t="s">
         <v>66</v>
       </c>
-      <c r="C254" s="34" t="s">
+      <c r="C254" s="149" t="s">
         <v>67</v>
       </c>
-      <c r="D254" s="35" t="s">
+      <c r="D254" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="E254" s="35">
+      <c r="E254" s="150">
         <v>2017</v>
       </c>
-      <c r="F254" s="34" t="s">
+      <c r="F254" s="149" t="s">
         <v>82</v>
       </c>
-      <c r="G254" s="34"/>
-      <c r="H254" s="34">
+      <c r="G254" s="149"/>
+      <c r="H254" s="149">
         <v>32</v>
       </c>
-      <c r="I254" s="34" t="s">
+      <c r="I254" s="149" t="s">
         <v>369</v>
       </c>
-      <c r="J254" s="34" t="s">
+      <c r="J254" s="149" t="s">
         <v>127</v>
       </c>
-      <c r="K254" s="34" t="s">
+      <c r="K254" s="149" t="s">
         <v>850</v>
       </c>
-      <c r="L254" s="72">
+      <c r="L254" s="151">
         <v>95</v>
       </c>
-      <c r="M254" s="129" t="s">
+      <c r="M254" s="141" t="s">
         <v>925</v>
       </c>
-      <c r="N254" s="34" t="s">
+      <c r="N254" s="149" t="s">
         <v>851</v>
       </c>
-      <c r="O254" s="132" t="s">
+      <c r="O254" s="142" t="s">
         <v>922</v>
       </c>
     </row>

</xml_diff>